<commit_message>
Fixed for Sari and Eme
</commit_message>
<xml_diff>
--- a/CsB tábor felvételi 2024 .xlsx
+++ b/CsB tábor felvételi 2024 .xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81b23c5e679c8043/MKK/CsBTábor2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="11_956C014C95CEDFDCDA2A6790F71A79149A918546" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36DEABC9-80EC-46D5-9735-CAF46EA8EBD7}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{C9A7EEC1-E01A-490E-92B9-46917EB4419E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D621E3CA-EDAA-44C9-9278-F11C4EBFD5FD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="450" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="271" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="A(z) 1. lapon lévő válaszok" sheetId="1" r:id="rId1"/>
+    <sheet name="CsB tábor felvételi 2024 " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="374">
   <si>
     <t>Időbélyeg</t>
   </si>
@@ -1145,6 +1145,153 @@
   </si>
   <si>
     <t>Kérdések</t>
+  </si>
+  <si>
+    <t>2024.08.14. 0:22:22</t>
+  </si>
+  <si>
+    <t>urbanyi.sara@gmail.com</t>
+  </si>
+  <si>
+    <t>Urbányi Sára</t>
+  </si>
+  <si>
+    <t>2001.04.24.</t>
+  </si>
+  <si>
+    <t>Jogász</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Tudjak repülni
+2. Legyek boldog az életben
+3. Legyen még 1M kívánságom.
+</t>
+  </si>
+  <si>
+    <t>1800-as évek végi Anglia. Női nemesi család egy tagja lennék, szép ruhákkal és sok bálra járnék.</t>
+  </si>
+  <si>
+    <t>Mulan, mert elszánt, kitartó, és meg akarja védeni a családját. Ja és nőként harcol a férfiak között…</t>
+  </si>
+  <si>
+    <t>Egyszer kiadatom egy regényem.</t>
+  </si>
+  <si>
+    <t>Türelem, mások véleményének elfogadása(kompromisszumkészség), szerénység</t>
+  </si>
+  <si>
+    <t>Kitartás, elhivatottság,őszinteség</t>
+  </si>
+  <si>
+    <t>Erőszakosság, hiúság, önzőség</t>
+  </si>
+  <si>
+    <t>Éhező gyerekek mindennap jóllakottan feküdjenek le.</t>
+  </si>
+  <si>
+    <t>Festés, orosz nyelv, szörfözés</t>
+  </si>
+  <si>
+    <t>Snowboard</t>
+  </si>
+  <si>
+    <t>Olvasás, naplóírás, úszás</t>
+  </si>
+  <si>
+    <t>Takarítás, focimeccs nézés, sütés(nem főzés;)</t>
+  </si>
+  <si>
+    <t>Föld összes országá tudom hol van, ezt szívesen megtanítom;)</t>
+  </si>
+  <si>
+    <t>Taylor Swift</t>
+  </si>
+  <si>
+    <t>Hogy két egyetemre járva tavaly januárban, 11 vizsgàból 1 kivételével mind 5 lett(azaz 1 meg négyes)</t>
+  </si>
+  <si>
+    <t>Hogy két egyetemre jártam miközben csopvez voltam.</t>
+  </si>
+  <si>
+    <t>Őszinteség.</t>
+  </si>
+  <si>
+    <t>Tdkt írni:(</t>
+  </si>
+  <si>
+    <t>Hogy soha ne akarjak megfelelni másoknak</t>
+  </si>
+  <si>
+    <t>Ha a barátaimmal lehetek.</t>
+  </si>
+  <si>
+    <t>Amikor a drága egyetlen barátom először megcsókolt&lt;3</t>
+  </si>
+  <si>
+    <t>Örökre 22</t>
+  </si>
+  <si>
+    <t>hála, optimizmus, őszinteség, bátorság, kíváncsiság, vezető képesség</t>
+  </si>
+  <si>
+    <t>2024.08.14. 15:24:32</t>
+  </si>
+  <si>
+    <t>vastag.mse@gmail.com</t>
+  </si>
+  <si>
+    <t>Vastag Emese</t>
+  </si>
+  <si>
+    <t>2000.10.29.</t>
+  </si>
+  <si>
+    <t>matematikus</t>
+  </si>
+  <si>
+    <t>Palacsinta</t>
+  </si>
+  <si>
+    <t>kitartás, türelem, határozottság</t>
+  </si>
+  <si>
+    <t>legyenek okosak, szeressenek olvasni, és legyenek önállóak</t>
+  </si>
+  <si>
+    <t>a szorgalmam (hiányát), az édesszájúságomat, a félénkségem</t>
+  </si>
+  <si>
+    <t>egymás elfogadása</t>
+  </si>
+  <si>
+    <t>magasabb szintű főzés</t>
+  </si>
+  <si>
+    <t>zongorázás</t>
+  </si>
+  <si>
+    <t>olvasás, sétálás, sütés</t>
+  </si>
+  <si>
+    <t>felmosás, hivatalos emailek írása, mosogatás</t>
+  </si>
+  <si>
+    <t>sütés</t>
+  </si>
+  <si>
+    <t>decibelszint növelése</t>
+  </si>
+  <si>
+    <t>olvasás/sorozatnézés</t>
+  </si>
+  <si>
+    <t>valamelyik nyaralás, egyszer voltam Prágában a húgaimmal és anyukámmal, vagy pedig amikor Horvátországban voltunk szintén a húgaimmal és barátokkal</t>
+  </si>
+  <si>
+    <t>20-23 között bármi</t>
+  </si>
+  <si>
+    <t>óvatosság, szépség értékelése, hála, őszinteség, ítélőképesség</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1301,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1188,6 +1335,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1209,7 +1370,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1217,29 +1378,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hivatkozás" xfId="1" builtinId="8"/>
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1253,10 +1470,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1460,1186 +1673,1403 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AI22"/>
+  <dimension ref="A1:AM22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="136" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="AE2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="AF16" sqref="AF16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26" customWidth="1"/>
-    <col min="5" max="5" width="73.85546875" customWidth="1"/>
-    <col min="6" max="6" width="46.5703125" customWidth="1"/>
-    <col min="7" max="7" width="147.5703125" customWidth="1"/>
-    <col min="8" max="39" width="18.85546875" customWidth="1"/>
+    <col min="1" max="2" width="18.85546875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="26" style="3" customWidth="1"/>
+    <col min="5" max="5" width="68.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="46.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="147.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="68.85546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="154.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.85546875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="125.85546875" style="3" customWidth="1"/>
+    <col min="12" max="12" width="78" style="3" customWidth="1"/>
+    <col min="13" max="13" width="69.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="83.7109375" style="3" customWidth="1"/>
+    <col min="15" max="15" width="71" style="3" customWidth="1"/>
+    <col min="16" max="16" width="67.140625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="72.85546875" style="3" customWidth="1"/>
+    <col min="18" max="18" width="41.42578125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="74.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="85.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="69.42578125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="87.42578125" style="3" customWidth="1"/>
+    <col min="23" max="23" width="112.140625" style="3" customWidth="1"/>
+    <col min="24" max="24" width="58.28515625" style="3" customWidth="1"/>
+    <col min="25" max="25" width="38.7109375" style="3" customWidth="1"/>
+    <col min="26" max="26" width="39.7109375" style="3" customWidth="1"/>
+    <col min="27" max="27" width="77.5703125" style="3" customWidth="1"/>
+    <col min="28" max="28" width="76.5703125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" style="3" customWidth="1"/>
+    <col min="30" max="30" width="41.28515625" style="3" customWidth="1"/>
+    <col min="31" max="31" width="59.7109375" style="3" customWidth="1"/>
+    <col min="32" max="32" width="75.5703125" style="3" customWidth="1"/>
+    <col min="33" max="39" width="18.85546875" style="3" customWidth="1"/>
+    <col min="40" max="16384" width="12.5703125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:39" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="V1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="Y1" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AC1" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="6" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="7"/>
-      <c r="AI1" s="7"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
     </row>
-    <row r="2" spans="1:35" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="2">
+    <row r="2" spans="1:39" ht="51" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="5">
         <v>45511.580394062505</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="D2" s="6">
         <v>36880</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="J2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="R2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="T2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="U2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="V2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="W2" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="X2" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AB2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AE2" s="1" t="s">
+      <c r="AE2" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AF2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5">
         <v>45511.54201704861</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D3" s="3">
+      <c r="D3" s="6">
         <v>36909</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="R3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="AC3" s="1" t="s">
+      <c r="AC3" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AF3" s="4">
         <v>18</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG3" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="5">
         <v>45511.549231053243</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="3">
+      <c r="D4" s="6">
         <v>36496</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="H4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="I4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="L4" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="N4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="O4" s="1" t="s">
+      <c r="O4" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="R4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="S4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="T4" s="1" t="s">
+      <c r="T4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="U4" s="1" t="s">
+      <c r="U4" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="V4" s="1" t="s">
+      <c r="V4" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="W4" s="1" t="s">
+      <c r="W4" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="X4" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="Y4" s="1" t="s">
+      <c r="Y4" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="Z4" s="1" t="s">
+      <c r="Z4" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AA4" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AB4" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="AC4" s="1" t="s">
+      <c r="AC4" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD4" s="1" t="s">
+      <c r="AD4" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="AE4" s="1" t="s">
+      <c r="AE4" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="AF4" s="1" t="s">
+      <c r="AF4" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="AG4" s="1" t="s">
+      <c r="AG4" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="5">
         <v>45511.55323193287</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="3">
+      <c r="D5" s="6">
         <v>36935</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="I5" s="1" t="s">
+      <c r="I5" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="K5" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="L5" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="N5" s="1" t="s">
+      <c r="N5" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="O5" s="1" t="s">
+      <c r="O5" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="R5" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="T5" s="1" t="s">
+      <c r="T5" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="U5" s="1" t="s">
+      <c r="U5" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="V5" s="1" t="s">
+      <c r="V5" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="W5" s="1" t="s">
+      <c r="W5" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="X5" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="Y5" s="1" t="s">
+      <c r="Y5" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="Z5" s="1" t="s">
+      <c r="Z5" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AA5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AB5" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="AC5" s="1" t="s">
+      <c r="AC5" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD5" s="1" t="s">
+      <c r="AD5" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="AE5" s="1" t="s">
+      <c r="AE5" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="AF5" s="1">
+      <c r="AF5" s="4">
         <v>20</v>
       </c>
-      <c r="AG5" s="1" t="s">
+      <c r="AG5" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="5">
         <v>45511.584193738425</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D6" s="3">
+      <c r="D6" s="6">
         <v>36875</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="K6" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="L6" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="N6" s="1" t="s">
+      <c r="N6" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O6" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="P6" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="Q6" s="1" t="s">
+      <c r="Q6" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="R6" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="S6" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="T6" s="1" t="s">
+      <c r="T6" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="U6" s="1" t="s">
+      <c r="U6" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="V6" s="1" t="s">
+      <c r="V6" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="W6" s="1" t="s">
+      <c r="W6" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="X6" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="Y6" s="1" t="s">
+      <c r="Y6" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="Z6" s="1" t="s">
+      <c r="Z6" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AA6" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AB6" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="AC6" s="1" t="s">
+      <c r="AC6" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD6" s="1" t="s">
+      <c r="AD6" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AE6" s="1" t="s">
+      <c r="AE6" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AF6" s="4">
         <v>24</v>
       </c>
-      <c r="AG6" s="1" t="s">
+      <c r="AG6" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:39" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="5">
         <v>45511.638691307875</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D7" s="3">
+      <c r="D7" s="6">
         <v>36644</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="J7" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="K7" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="M7" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="N7" s="1" t="s">
+      <c r="N7" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="O7" s="1" t="s">
+      <c r="O7" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="P7" s="1" t="s">
+      <c r="P7" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="Q7" s="1" t="s">
+      <c r="Q7" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="R7" s="1" t="s">
+      <c r="R7" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="S7" s="1" t="s">
+      <c r="S7" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="T7" s="1" t="s">
+      <c r="T7" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="U7" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="V7" s="1" t="s">
+      <c r="V7" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="W7" s="1" t="s">
+      <c r="W7" s="4" t="s">
         <v>179</v>
       </c>
-      <c r="X7" s="1" t="s">
+      <c r="X7" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="Y7" s="1" t="s">
+      <c r="Y7" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="Z7" s="1" t="s">
+      <c r="Z7" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AA7" s="4" t="s">
         <v>183</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AB7" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="AC7" s="1" t="s">
+      <c r="AC7" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD7" s="1" t="s">
+      <c r="AD7" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="AE7" s="1" t="s">
+      <c r="AE7" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="AF7" s="1">
+      <c r="AF7" s="4">
         <v>100</v>
       </c>
-      <c r="AG7" s="1" t="s">
+      <c r="AG7" s="4" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="8" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" s="5">
         <v>45511.75867304398</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="3">
+      <c r="D8" s="6">
         <v>36879</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="M8" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="N8" s="1" t="s">
+      <c r="N8" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="O8" s="1" t="s">
+      <c r="O8" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="P8" s="1" t="s">
+      <c r="P8" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="Q8" s="1" t="s">
+      <c r="Q8" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="R8" s="1" t="s">
+      <c r="R8" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="S8" s="1" t="s">
+      <c r="S8" s="4" t="s">
         <v>204</v>
       </c>
-      <c r="T8" s="1" t="s">
+      <c r="T8" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="U8" s="4" t="s">
         <v>206</v>
       </c>
-      <c r="V8" s="1" t="s">
+      <c r="V8" s="4" t="s">
         <v>207</v>
       </c>
-      <c r="W8" s="1" t="s">
+      <c r="W8" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="X8" s="1" t="s">
+      <c r="X8" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="Z8" s="1" t="s">
+      <c r="Z8" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AA8" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AB8" s="4" t="s">
         <v>212</v>
       </c>
-      <c r="AC8" s="1" t="s">
+      <c r="AC8" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD8" s="1" t="s">
+      <c r="AD8" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="AE8" s="1" t="s">
+      <c r="AE8" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="AF8" s="1">
+      <c r="AF8" s="4">
         <v>20</v>
       </c>
-      <c r="AG8" s="1" t="s">
+      <c r="AG8" s="4" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="5">
         <v>45514.350220960652</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="D9" s="3">
+      <c r="D9" s="6">
         <v>36644</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="8" t="s">
         <v>221</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="I9" s="8" t="s">
         <v>222</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="L9" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="M9" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="N9" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="O9" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="R9" s="1" t="s">
+      <c r="R9" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="S9" s="1" t="s">
+      <c r="S9" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="T9" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="U9" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="V9" s="1" t="s">
+      <c r="V9" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="W9" s="1" t="s">
+      <c r="W9" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="X9" s="1" t="s">
+      <c r="X9" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AB9" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="AC9" s="1" t="s">
+      <c r="AC9" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AD9" s="1" t="s">
+      <c r="AD9" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="AE9" s="1" t="s">
+      <c r="AE9" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="AF9" s="1" t="s">
+      <c r="AF9" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="AG9" s="1" t="s">
+      <c r="AG9" s="4" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="10" spans="1:35" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:39" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B10" s="5">
         <v>45515.888268773153</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" s="3">
+      <c r="D10" s="6">
         <v>36177</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="8" t="s">
         <v>245</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G10" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="H10" s="1" t="s">
+      <c r="H10" s="8" t="s">
         <v>247</v>
       </c>
-      <c r="I10" s="1"/>
-      <c r="K10" s="1" t="s">
+      <c r="I10" s="4"/>
+      <c r="K10" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="M10" s="4" t="s">
         <v>250</v>
       </c>
-      <c r="N10" s="1" t="s">
+      <c r="N10" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="O10" s="1" t="s">
+      <c r="O10" s="8" t="s">
         <v>252</v>
       </c>
-      <c r="P10" s="1" t="s">
+      <c r="P10" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="Q10" s="1" t="s">
+      <c r="Q10" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="R10" s="1" t="s">
+      <c r="R10" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="S10" s="1" t="s">
+      <c r="S10" s="4" t="s">
         <v>256</v>
       </c>
-      <c r="T10" s="1" t="s">
+      <c r="T10" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="U10" s="1" t="s">
+      <c r="U10" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="V10" s="1" t="s">
+      <c r="V10" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="W10" s="1" t="s">
+      <c r="W10" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="Y10" s="1" t="s">
+      <c r="Y10" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="Z10" s="1" t="s">
+      <c r="Z10" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AA10" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AB10" s="8" t="s">
         <v>264</v>
       </c>
-      <c r="AC10" s="1" t="s">
+      <c r="AC10" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD10" s="1" t="s">
+      <c r="AD10" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="AF10" s="1" t="s">
+      <c r="AF10" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="AG10" s="1" t="s">
+      <c r="AG10" s="4" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:39" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="5">
         <v>45516.379143819446</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="D11" s="6">
         <v>36273</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="H11" s="1" t="s">
+      <c r="H11" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="4" t="s">
         <v>276</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="4" t="s">
         <v>278</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="S11" s="1" t="s">
+      <c r="S11" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="T11" s="1" t="s">
+      <c r="T11" s="4" t="s">
         <v>282</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="U11" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="V11" s="1" t="s">
+      <c r="V11" s="4" t="s">
         <v>284</v>
       </c>
-      <c r="X11" s="1" t="s">
+      <c r="X11" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="Z11" s="1" t="s">
+      <c r="Z11" s="4" t="s">
         <v>286</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AA11" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AB11" s="4" t="s">
         <v>288</v>
       </c>
-      <c r="AC11" s="1" t="s">
+      <c r="AC11" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="AD11" s="1" t="s">
+      <c r="AD11" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="AE11" s="1" t="s">
+      <c r="AE11" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="AF11" s="1">
+      <c r="AF11" s="4">
         <v>23</v>
       </c>
-      <c r="AG11" s="1" t="s">
+      <c r="AG11" s="4" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:39" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="5">
         <v>45516.591501724542</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="D12" s="3">
+      <c r="D12" s="6">
         <v>37173</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="4" t="s">
         <v>296</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="8" t="s">
         <v>298</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="4" t="s">
         <v>302</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="N12" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="O12" s="8" t="s">
         <v>304</v>
       </c>
-      <c r="P12" s="1" t="s">
+      <c r="P12" s="4" t="s">
         <v>305</v>
       </c>
-      <c r="Q12" s="1" t="s">
+      <c r="Q12" s="4" t="s">
         <v>306</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="S12" s="1" t="s">
+      <c r="S12" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="T12" s="1" t="s">
+      <c r="T12" s="4" t="s">
         <v>309</v>
       </c>
-      <c r="U12" s="1" t="s">
+      <c r="U12" s="4" t="s">
         <v>310</v>
       </c>
-      <c r="V12" s="1" t="s">
+      <c r="V12" s="4" t="s">
         <v>311</v>
       </c>
-      <c r="W12" s="1" t="s">
+      <c r="W12" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="X12" s="1" t="s">
+      <c r="X12" s="8" t="s">
         <v>313</v>
       </c>
-      <c r="Z12" s="1" t="s">
+      <c r="Z12" s="8" t="s">
         <v>314</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AA12" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AB12" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="AC12" s="1" t="s">
+      <c r="AC12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AD12" s="1" t="s">
+      <c r="AD12" s="4" t="s">
         <v>317</v>
       </c>
-      <c r="AE12" s="1" t="s">
+      <c r="AE12" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="AF12" s="1" t="s">
+      <c r="AF12" s="4" t="s">
         <v>319</v>
       </c>
-      <c r="AG12" s="1" t="s">
+      <c r="AG12" s="4" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="15" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D15" s="7" t="s">
+    <row r="13" spans="1:39" ht="37.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>326</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>327</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>330</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>332</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>334</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="M13" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="Q13" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="S13" s="4" t="s">
+        <v>342</v>
+      </c>
+      <c r="T13" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="U13" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="V13" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="W13" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="X13" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4" t="s">
+        <v>348</v>
+      </c>
+      <c r="AA13" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="AB13" s="4"/>
+      <c r="AC13" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD13" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="AE13" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="AF13" s="4" t="s">
+        <v>352</v>
+      </c>
+      <c r="AG13" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="16"/>
+      <c r="AK13" s="16"/>
+      <c r="AL13" s="16"/>
+      <c r="AM13" s="16"/>
+    </row>
+    <row r="14" spans="1:39" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>354</v>
+      </c>
+      <c r="C14" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>358</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="M14" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="N14" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q14" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="S14" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="T14" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="4"/>
+      <c r="X14" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="Y14" s="4"/>
+      <c r="Z14" s="4"/>
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4"/>
+      <c r="AC14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD14" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="AE14" s="8" t="s">
+        <v>371</v>
+      </c>
+      <c r="AF14" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="AG14" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="AH14" s="4"/>
+      <c r="AI14" s="4"/>
+      <c r="AJ14" s="16"/>
+      <c r="AK14" s="16"/>
+      <c r="AL14" s="16"/>
+      <c r="AM14" s="16"/>
+    </row>
+    <row r="15" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D15" s="2" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D16" t="s">
+    <row r="16" spans="1:39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D16" s="3" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="5">
+    <row r="17" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D17" s="11">
         <f>MAX(D2:D12)</f>
         <v>37173</v>
       </c>
     </row>
-    <row r="18" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D18" s="7" t="s">
+    <row r="18" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D18" s="2" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="19" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D19" t="s">
+    <row r="19" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D19" s="3" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D20" s="5">
+    <row r="20" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D20" s="11">
         <f>MIN(D2:D12)</f>
         <v>36177</v>
       </c>
     </row>
-    <row r="22" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="8" t="s">
+    <row r="22" spans="3:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C22" s="12" t="s">
         <v>325</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="O6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C13" r:id="rId2" xr:uid="{7F47B2F3-92C2-4D2A-B992-0FACF3136CCD}"/>
+    <hyperlink ref="C14" r:id="rId3" xr:uid="{051E65EB-8F86-42EC-8410-23ED13291F1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId2"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>